<commit_message>
?????????? ?????? ? ???????, ???? ??? ???????? ??? ?????????. ? ??? ?? ?? ?????????? ?????????, ???? ??? (?????) ??????????? ? ??????.
</commit_message>
<xml_diff>
--- a/src/tests/test_data/linux/test-PF_PKO.xlsx
+++ b/src/tests/test_data/linux/test-PF_PKO.xlsx
@@ -393,12 +393,13 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="5">
+  <numFmts count="6">
     <numFmt formatCode="GENERAL" numFmtId="164"/>
     <numFmt formatCode="@" numFmtId="165"/>
     <numFmt formatCode="DD\/MM\/YY" numFmtId="166"/>
-    <numFmt formatCode="0.00_ ;[RED]\-0.00\ " numFmtId="167"/>
-    <numFmt formatCode="#,##0_ ;[RED]\-#,##0\ " numFmtId="168"/>
+    <numFmt formatCode="#,##0.00;[RED]\-#,##0.00" numFmtId="167"/>
+    <numFmt formatCode="0.00_ ;[RED]\-0.00\ " numFmtId="168"/>
+    <numFmt formatCode="#,##0_ ;[RED]\-#,##0\ " numFmtId="169"/>
   </numFmts>
   <fonts count="16">
     <font>
@@ -637,7 +638,7 @@
     <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="42"/>
     <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="9"/>
   </cellStyleXfs>
-  <cellXfs count="84">
+  <cellXfs count="85">
     <xf applyAlignment="false" applyBorder="false" applyFont="false" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="164" xfId="0"/>
     <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="4" numFmtId="164" xfId="0">
       <alignment horizontal="center" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
@@ -787,6 +788,9 @@
       <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
     </xf>
     <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="165" xfId="0"/>
+    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="false" borderId="7" fillId="2" fontId="4" numFmtId="168" xfId="0">
+      <alignment horizontal="center" indent="0" shrinkToFit="false" textRotation="0" vertical="center" wrapText="false"/>
+    </xf>
     <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="false" borderId="1" fillId="0" fontId="11" numFmtId="164" xfId="0">
       <alignment horizontal="center" indent="0" shrinkToFit="false" textRotation="0" vertical="distributed" wrapText="true"/>
     </xf>
@@ -799,7 +803,7 @@
     <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="false" borderId="4" fillId="0" fontId="4" numFmtId="164" xfId="0">
       <alignment horizontal="right" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
     </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="false" borderId="6" fillId="2" fontId="4" numFmtId="168" xfId="0">
+    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="false" borderId="6" fillId="2" fontId="4" numFmtId="169" xfId="0">
       <alignment horizontal="right" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
     </xf>
     <xf applyAlignment="true" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="4" numFmtId="164" xfId="0">
@@ -887,30 +891,30 @@
   </sheetPr>
   <dimension ref="A1:DM41"/>
   <sheetViews>
-    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <pane activePane="topLeft" topLeftCell="A1" xSplit="0" ySplit="-1"/>
-      <selection activeCell="A1" activeCellId="0" pane="topLeft" sqref="A1"/>
-      <selection activeCell="A1" activeCellId="0" pane="bottomLeft" sqref="A1"/>
+    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A4" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
+      <pane activePane="topLeft" topLeftCell="A4" xSplit="0" ySplit="-1"/>
+      <selection activeCell="AL21" activeCellId="0" pane="topLeft" sqref="AL21"/>
+      <selection activeCell="A4" activeCellId="0" pane="bottomLeft" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <cols>
     <col collapsed="false" hidden="false" max="2" min="1" style="0" width="1.01176470588235"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="1.43921568627451"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="1.45490196078431"/>
     <col collapsed="false" hidden="false" max="10" min="4" style="0" width="1.01176470588235"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="2.0156862745098"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="2.03529411764706"/>
     <col collapsed="false" hidden="false" max="12" min="12" style="0" width="1.01176470588235"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="2.0156862745098"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="2.03529411764706"/>
     <col collapsed="false" hidden="false" max="27" min="14" style="0" width="1.01176470588235"/>
-    <col collapsed="false" hidden="false" max="28" min="28" style="0" width="2.0156862745098"/>
-    <col collapsed="false" hidden="false" max="29" min="29" style="0" width="1.87058823529412"/>
+    <col collapsed="false" hidden="false" max="28" min="28" style="0" width="2.03529411764706"/>
+    <col collapsed="false" hidden="false" max="29" min="29" style="0" width="1.89019607843137"/>
     <col collapsed="false" hidden="false" max="80" min="30" style="0" width="1.01176470588235"/>
-    <col collapsed="false" hidden="false" max="81" min="81" style="0" width="2.0156862745098"/>
-    <col collapsed="false" hidden="false" max="82" min="82" style="0" width="1.30196078431373"/>
+    <col collapsed="false" hidden="false" max="81" min="81" style="0" width="2.03529411764706"/>
+    <col collapsed="false" hidden="false" max="82" min="82" style="0" width="1.32156862745098"/>
     <col collapsed="false" hidden="false" max="111" min="83" style="0" width="1.01176470588235"/>
-    <col collapsed="false" hidden="false" max="112" min="112" style="0" width="5.76078431372549"/>
+    <col collapsed="false" hidden="false" max="112" min="112" style="0" width="5.8156862745098"/>
     <col collapsed="false" hidden="false" max="113" min="113" style="0" width="1.01176470588235"/>
-    <col collapsed="false" hidden="false" max="114" min="114" style="0" width="10.5176470588235"/>
-    <col collapsed="false" hidden="false" max="1025" min="115" style="0" width="11.6666666666667"/>
+    <col collapsed="false" hidden="false" max="114" min="114" style="0" width="10.6196078431373"/>
+    <col collapsed="false" hidden="false" max="1025" min="115" style="0" width="11.7843137254902"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="true" customHeight="true" hidden="false" ht="10.5" outlineLevel="0" r="1" s="7">
@@ -3441,17 +3445,17 @@
       <c r="AI21" s="51"/>
       <c r="AJ21" s="51"/>
       <c r="AK21" s="51"/>
-      <c r="AL21" s="50" t="s">
+      <c r="AL21" s="52" t="s">
         <v>69</v>
       </c>
-      <c r="AM21" s="50"/>
-      <c r="AN21" s="50"/>
-      <c r="AO21" s="50"/>
-      <c r="AP21" s="50"/>
-      <c r="AQ21" s="50"/>
-      <c r="AR21" s="50"/>
-      <c r="AS21" s="50"/>
-      <c r="AT21" s="50"/>
+      <c r="AM21" s="52"/>
+      <c r="AN21" s="52"/>
+      <c r="AO21" s="52"/>
+      <c r="AP21" s="52"/>
+      <c r="AQ21" s="52"/>
+      <c r="AR21" s="52"/>
+      <c r="AS21" s="52"/>
+      <c r="AT21" s="52"/>
       <c r="AU21" s="52" t="s">
         <v>70</v>
       </c>
@@ -3577,17 +3581,17 @@
       <c r="AR22" s="50"/>
       <c r="AS22" s="50"/>
       <c r="AT22" s="50"/>
-      <c r="AU22" s="52"/>
-      <c r="AV22" s="52"/>
-      <c r="AW22" s="52"/>
-      <c r="AX22" s="52"/>
-      <c r="AY22" s="52"/>
-      <c r="AZ22" s="52"/>
-      <c r="BA22" s="52"/>
-      <c r="BB22" s="52"/>
-      <c r="BC22" s="52"/>
-      <c r="BD22" s="52"/>
-      <c r="BE22" s="52"/>
+      <c r="AU22" s="57"/>
+      <c r="AV22" s="57"/>
+      <c r="AW22" s="57"/>
+      <c r="AX22" s="57"/>
+      <c r="AY22" s="57"/>
+      <c r="AZ22" s="57"/>
+      <c r="BA22" s="57"/>
+      <c r="BB22" s="57"/>
+      <c r="BC22" s="57"/>
+      <c r="BD22" s="57"/>
+      <c r="BE22" s="57"/>
       <c r="BF22" s="50"/>
       <c r="BG22" s="50"/>
       <c r="BH22" s="50"/>
@@ -3648,133 +3652,133 @@
         <v>74</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="true" customHeight="true" hidden="false" ht="12" outlineLevel="0" r="23" s="68">
-      <c r="A23" s="57"/>
-      <c r="B23" s="57"/>
-      <c r="C23" s="57"/>
-      <c r="D23" s="57"/>
-      <c r="E23" s="57"/>
-      <c r="F23" s="57"/>
-      <c r="G23" s="57"/>
-      <c r="H23" s="57"/>
-      <c r="I23" s="57"/>
-      <c r="J23" s="57"/>
-      <c r="K23" s="57"/>
-      <c r="L23" s="57"/>
-      <c r="M23" s="57"/>
-      <c r="N23" s="57"/>
-      <c r="O23" s="57"/>
-      <c r="P23" s="57"/>
-      <c r="Q23" s="57"/>
-      <c r="R23" s="57"/>
-      <c r="S23" s="57"/>
-      <c r="T23" s="57"/>
-      <c r="U23" s="57"/>
-      <c r="V23" s="57"/>
-      <c r="W23" s="57"/>
-      <c r="X23" s="57"/>
-      <c r="Y23" s="57"/>
-      <c r="Z23" s="57"/>
-      <c r="AA23" s="57"/>
-      <c r="AB23" s="57"/>
-      <c r="AC23" s="57"/>
-      <c r="AD23" s="57"/>
-      <c r="AE23" s="57"/>
-      <c r="AF23" s="57"/>
-      <c r="AG23" s="57"/>
-      <c r="AH23" s="57"/>
-      <c r="AI23" s="57"/>
-      <c r="AJ23" s="57"/>
-      <c r="AK23" s="57"/>
-      <c r="AL23" s="57"/>
-      <c r="AM23" s="57"/>
-      <c r="AN23" s="57"/>
-      <c r="AO23" s="57"/>
-      <c r="AP23" s="57"/>
-      <c r="AQ23" s="57"/>
-      <c r="AR23" s="57"/>
-      <c r="AS23" s="57"/>
-      <c r="AT23" s="57"/>
-      <c r="AU23" s="57"/>
-      <c r="AV23" s="57"/>
-      <c r="AW23" s="57"/>
-      <c r="AX23" s="57"/>
-      <c r="AY23" s="57"/>
-      <c r="AZ23" s="57"/>
-      <c r="BA23" s="57"/>
-      <c r="BB23" s="57"/>
-      <c r="BC23" s="57"/>
-      <c r="BD23" s="57"/>
-      <c r="BE23" s="57"/>
-      <c r="BF23" s="57"/>
-      <c r="BG23" s="57"/>
-      <c r="BH23" s="57"/>
-      <c r="BI23" s="57"/>
-      <c r="BJ23" s="57"/>
-      <c r="BK23" s="57"/>
-      <c r="BL23" s="57"/>
-      <c r="BM23" s="57"/>
-      <c r="BN23" s="57"/>
-      <c r="BO23" s="57"/>
-      <c r="BP23" s="57"/>
-      <c r="BQ23" s="58" t="s">
+    <row collapsed="false" customFormat="true" customHeight="true" hidden="false" ht="12" outlineLevel="0" r="23" s="69">
+      <c r="A23" s="58"/>
+      <c r="B23" s="58"/>
+      <c r="C23" s="58"/>
+      <c r="D23" s="58"/>
+      <c r="E23" s="58"/>
+      <c r="F23" s="58"/>
+      <c r="G23" s="58"/>
+      <c r="H23" s="58"/>
+      <c r="I23" s="58"/>
+      <c r="J23" s="58"/>
+      <c r="K23" s="58"/>
+      <c r="L23" s="58"/>
+      <c r="M23" s="58"/>
+      <c r="N23" s="58"/>
+      <c r="O23" s="58"/>
+      <c r="P23" s="58"/>
+      <c r="Q23" s="58"/>
+      <c r="R23" s="58"/>
+      <c r="S23" s="58"/>
+      <c r="T23" s="58"/>
+      <c r="U23" s="58"/>
+      <c r="V23" s="58"/>
+      <c r="W23" s="58"/>
+      <c r="X23" s="58"/>
+      <c r="Y23" s="58"/>
+      <c r="Z23" s="58"/>
+      <c r="AA23" s="58"/>
+      <c r="AB23" s="58"/>
+      <c r="AC23" s="58"/>
+      <c r="AD23" s="58"/>
+      <c r="AE23" s="58"/>
+      <c r="AF23" s="58"/>
+      <c r="AG23" s="58"/>
+      <c r="AH23" s="58"/>
+      <c r="AI23" s="58"/>
+      <c r="AJ23" s="58"/>
+      <c r="AK23" s="58"/>
+      <c r="AL23" s="58"/>
+      <c r="AM23" s="58"/>
+      <c r="AN23" s="58"/>
+      <c r="AO23" s="58"/>
+      <c r="AP23" s="58"/>
+      <c r="AQ23" s="58"/>
+      <c r="AR23" s="58"/>
+      <c r="AS23" s="58"/>
+      <c r="AT23" s="58"/>
+      <c r="AU23" s="58"/>
+      <c r="AV23" s="58"/>
+      <c r="AW23" s="58"/>
+      <c r="AX23" s="58"/>
+      <c r="AY23" s="58"/>
+      <c r="AZ23" s="58"/>
+      <c r="BA23" s="58"/>
+      <c r="BB23" s="58"/>
+      <c r="BC23" s="58"/>
+      <c r="BD23" s="58"/>
+      <c r="BE23" s="58"/>
+      <c r="BF23" s="58"/>
+      <c r="BG23" s="58"/>
+      <c r="BH23" s="58"/>
+      <c r="BI23" s="58"/>
+      <c r="BJ23" s="58"/>
+      <c r="BK23" s="58"/>
+      <c r="BL23" s="58"/>
+      <c r="BM23" s="58"/>
+      <c r="BN23" s="58"/>
+      <c r="BO23" s="58"/>
+      <c r="BP23" s="58"/>
+      <c r="BQ23" s="59" t="s">
         <v>75</v>
       </c>
-      <c r="BR23" s="58"/>
-      <c r="BS23" s="59"/>
-      <c r="BT23" s="60" t="s">
+      <c r="BR23" s="59"/>
+      <c r="BS23" s="60"/>
+      <c r="BT23" s="61" t="s">
         <v>76</v>
       </c>
-      <c r="BU23" s="60"/>
-      <c r="BV23" s="60"/>
-      <c r="BW23" s="60"/>
-      <c r="BX23" s="60"/>
-      <c r="BY23" s="60"/>
-      <c r="BZ23" s="60"/>
-      <c r="CA23" s="61" t="s">
+      <c r="BU23" s="61"/>
+      <c r="BV23" s="61"/>
+      <c r="BW23" s="61"/>
+      <c r="BX23" s="61"/>
+      <c r="BY23" s="61"/>
+      <c r="BZ23" s="61"/>
+      <c r="CA23" s="62" t="s">
         <v>77</v>
       </c>
-      <c r="CB23" s="61"/>
-      <c r="CC23" s="61"/>
-      <c r="CD23" s="61"/>
-      <c r="CE23" s="61"/>
-      <c r="CF23" s="61"/>
-      <c r="CG23" s="61"/>
-      <c r="CH23" s="61"/>
-      <c r="CI23" s="61"/>
-      <c r="CJ23" s="61"/>
-      <c r="CK23" s="61"/>
-      <c r="CL23" s="61"/>
-      <c r="CM23" s="61"/>
-      <c r="CN23" s="61"/>
-      <c r="CO23" s="61"/>
-      <c r="CP23" s="61"/>
-      <c r="CQ23" s="61"/>
-      <c r="CR23" s="62"/>
-      <c r="CS23" s="63" t="s">
+      <c r="CB23" s="62"/>
+      <c r="CC23" s="62"/>
+      <c r="CD23" s="62"/>
+      <c r="CE23" s="62"/>
+      <c r="CF23" s="62"/>
+      <c r="CG23" s="62"/>
+      <c r="CH23" s="62"/>
+      <c r="CI23" s="62"/>
+      <c r="CJ23" s="62"/>
+      <c r="CK23" s="62"/>
+      <c r="CL23" s="62"/>
+      <c r="CM23" s="62"/>
+      <c r="CN23" s="62"/>
+      <c r="CO23" s="62"/>
+      <c r="CP23" s="62"/>
+      <c r="CQ23" s="62"/>
+      <c r="CR23" s="63"/>
+      <c r="CS23" s="64" t="s">
         <v>78</v>
       </c>
-      <c r="CT23" s="62"/>
-      <c r="CU23" s="64"/>
-      <c r="CV23" s="64"/>
-      <c r="CW23" s="65" t="s">
+      <c r="CT23" s="63"/>
+      <c r="CU23" s="65"/>
+      <c r="CV23" s="65"/>
+      <c r="CW23" s="66" t="s">
         <v>79</v>
       </c>
-      <c r="CX23" s="65"/>
-      <c r="CY23" s="65"/>
-      <c r="CZ23" s="65"/>
-      <c r="DA23" s="65"/>
-      <c r="DB23" s="62" t="s">
+      <c r="CX23" s="66"/>
+      <c r="CY23" s="66"/>
+      <c r="CZ23" s="66"/>
+      <c r="DA23" s="66"/>
+      <c r="DB23" s="63" t="s">
         <v>80</v>
       </c>
-      <c r="DC23" s="62"/>
-      <c r="DD23" s="62"/>
-      <c r="DE23" s="62"/>
-      <c r="DF23" s="66"/>
-      <c r="DG23" s="67"/>
-      <c r="DH23" s="67"/>
-      <c r="DI23" s="66"/>
-      <c r="DL23" s="69"/>
+      <c r="DC23" s="63"/>
+      <c r="DD23" s="63"/>
+      <c r="DE23" s="63"/>
+      <c r="DF23" s="67"/>
+      <c r="DG23" s="68"/>
+      <c r="DH23" s="68"/>
+      <c r="DI23" s="67"/>
+      <c r="DL23" s="70"/>
     </row>
     <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="24" s="7">
       <c r="A24" s="11"/>
@@ -3845,8 +3849,8 @@
       <c r="BN24" s="11"/>
       <c r="BO24" s="11"/>
       <c r="BP24" s="11"/>
-      <c r="BQ24" s="58"/>
-      <c r="BR24" s="58"/>
+      <c r="BQ24" s="59"/>
+      <c r="BR24" s="59"/>
       <c r="BS24" s="12"/>
       <c r="BT24" s="13"/>
       <c r="BU24" s="13"/>
@@ -3855,25 +3859,25 @@
       <c r="BX24" s="13"/>
       <c r="BY24" s="13"/>
       <c r="BZ24" s="13"/>
-      <c r="CA24" s="70" t="s">
+      <c r="CA24" s="71" t="s">
         <v>81</v>
       </c>
-      <c r="CB24" s="70"/>
-      <c r="CC24" s="70"/>
-      <c r="CD24" s="70"/>
-      <c r="CE24" s="70"/>
-      <c r="CF24" s="70"/>
-      <c r="CG24" s="70"/>
-      <c r="CH24" s="70"/>
-      <c r="CI24" s="70"/>
-      <c r="CJ24" s="70"/>
-      <c r="CK24" s="70"/>
-      <c r="CL24" s="70"/>
-      <c r="CM24" s="70"/>
-      <c r="CN24" s="70"/>
-      <c r="CO24" s="70"/>
-      <c r="CP24" s="70"/>
-      <c r="CQ24" s="70"/>
+      <c r="CB24" s="71"/>
+      <c r="CC24" s="71"/>
+      <c r="CD24" s="71"/>
+      <c r="CE24" s="71"/>
+      <c r="CF24" s="71"/>
+      <c r="CG24" s="71"/>
+      <c r="CH24" s="71"/>
+      <c r="CI24" s="71"/>
+      <c r="CJ24" s="71"/>
+      <c r="CK24" s="71"/>
+      <c r="CL24" s="71"/>
+      <c r="CM24" s="71"/>
+      <c r="CN24" s="71"/>
+      <c r="CO24" s="71"/>
+      <c r="CP24" s="71"/>
+      <c r="CQ24" s="71"/>
       <c r="CR24" s="22"/>
       <c r="CS24" s="22"/>
       <c r="CT24" s="22"/>
@@ -3967,8 +3971,8 @@
       <c r="BN25" s="34"/>
       <c r="BO25" s="34"/>
       <c r="BP25" s="16"/>
-      <c r="BQ25" s="58"/>
-      <c r="BR25" s="58"/>
+      <c r="BQ25" s="59"/>
+      <c r="BR25" s="59"/>
       <c r="BS25" s="4"/>
       <c r="BT25" s="6"/>
       <c r="BU25" s="34" t="s">
@@ -4085,130 +4089,130 @@
       <c r="BN26" s="22"/>
       <c r="BO26" s="22"/>
       <c r="BP26" s="24"/>
-      <c r="BQ26" s="58"/>
-      <c r="BR26" s="58"/>
+      <c r="BQ26" s="59"/>
+      <c r="BR26" s="59"/>
       <c r="BS26" s="12"/>
       <c r="BT26" s="6"/>
-      <c r="BU26" s="70" t="s">
+      <c r="BU26" s="71" t="s">
         <v>83</v>
       </c>
-      <c r="BV26" s="70"/>
-      <c r="BW26" s="70"/>
-      <c r="BX26" s="70"/>
-      <c r="BY26" s="70"/>
-      <c r="BZ26" s="70"/>
-      <c r="CA26" s="70"/>
-      <c r="CB26" s="70"/>
-      <c r="CC26" s="70"/>
-      <c r="CD26" s="70"/>
-      <c r="CE26" s="70"/>
-      <c r="CF26" s="70"/>
-      <c r="CG26" s="70"/>
-      <c r="CH26" s="70"/>
-      <c r="CI26" s="70"/>
-      <c r="CJ26" s="70"/>
-      <c r="CK26" s="70"/>
-      <c r="CL26" s="70"/>
-      <c r="CM26" s="70"/>
-      <c r="CN26" s="70"/>
-      <c r="CO26" s="70"/>
-      <c r="CP26" s="70"/>
-      <c r="CQ26" s="70"/>
-      <c r="CR26" s="70"/>
-      <c r="CS26" s="70"/>
-      <c r="CT26" s="70"/>
-      <c r="CU26" s="70"/>
-      <c r="CV26" s="70"/>
-      <c r="CW26" s="70"/>
-      <c r="CX26" s="70"/>
-      <c r="CY26" s="70"/>
-      <c r="CZ26" s="70"/>
-      <c r="DA26" s="70"/>
-      <c r="DB26" s="70"/>
-      <c r="DC26" s="70"/>
-      <c r="DD26" s="70"/>
-      <c r="DE26" s="70"/>
-      <c r="DF26" s="70"/>
-      <c r="DG26" s="70"/>
-      <c r="DH26" s="70"/>
+      <c r="BV26" s="71"/>
+      <c r="BW26" s="71"/>
+      <c r="BX26" s="71"/>
+      <c r="BY26" s="71"/>
+      <c r="BZ26" s="71"/>
+      <c r="CA26" s="71"/>
+      <c r="CB26" s="71"/>
+      <c r="CC26" s="71"/>
+      <c r="CD26" s="71"/>
+      <c r="CE26" s="71"/>
+      <c r="CF26" s="71"/>
+      <c r="CG26" s="71"/>
+      <c r="CH26" s="71"/>
+      <c r="CI26" s="71"/>
+      <c r="CJ26" s="71"/>
+      <c r="CK26" s="71"/>
+      <c r="CL26" s="71"/>
+      <c r="CM26" s="71"/>
+      <c r="CN26" s="71"/>
+      <c r="CO26" s="71"/>
+      <c r="CP26" s="71"/>
+      <c r="CQ26" s="71"/>
+      <c r="CR26" s="71"/>
+      <c r="CS26" s="71"/>
+      <c r="CT26" s="71"/>
+      <c r="CU26" s="71"/>
+      <c r="CV26" s="71"/>
+      <c r="CW26" s="71"/>
+      <c r="CX26" s="71"/>
+      <c r="CY26" s="71"/>
+      <c r="CZ26" s="71"/>
+      <c r="DA26" s="71"/>
+      <c r="DB26" s="71"/>
+      <c r="DC26" s="71"/>
+      <c r="DD26" s="71"/>
+      <c r="DE26" s="71"/>
+      <c r="DF26" s="71"/>
+      <c r="DG26" s="71"/>
+      <c r="DH26" s="71"/>
       <c r="DI26" s="6"/>
       <c r="DL26" s="8"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="10.5" outlineLevel="0" r="27">
       <c r="A27" s="6"/>
-      <c r="B27" s="62" t="s">
+      <c r="B27" s="63" t="s">
         <v>84</v>
       </c>
-      <c r="C27" s="62"/>
-      <c r="D27" s="62"/>
-      <c r="E27" s="62"/>
-      <c r="F27" s="62"/>
-      <c r="G27" s="62"/>
-      <c r="H27" s="62"/>
-      <c r="I27" s="62"/>
-      <c r="J27" s="62"/>
-      <c r="K27" s="62"/>
-      <c r="L27" s="71" t="s">
+      <c r="C27" s="63"/>
+      <c r="D27" s="63"/>
+      <c r="E27" s="63"/>
+      <c r="F27" s="63"/>
+      <c r="G27" s="63"/>
+      <c r="H27" s="63"/>
+      <c r="I27" s="63"/>
+      <c r="J27" s="63"/>
+      <c r="K27" s="63"/>
+      <c r="L27" s="72" t="s">
         <v>54</v>
       </c>
-      <c r="M27" s="71"/>
-      <c r="N27" s="71"/>
-      <c r="O27" s="71"/>
-      <c r="P27" s="71"/>
-      <c r="Q27" s="71"/>
-      <c r="R27" s="71"/>
-      <c r="S27" s="71"/>
-      <c r="T27" s="71"/>
-      <c r="U27" s="71"/>
-      <c r="V27" s="71"/>
-      <c r="W27" s="71"/>
-      <c r="X27" s="71"/>
-      <c r="Y27" s="71"/>
-      <c r="Z27" s="71"/>
-      <c r="AA27" s="71"/>
-      <c r="AB27" s="71"/>
-      <c r="AC27" s="71"/>
-      <c r="AD27" s="71"/>
-      <c r="AE27" s="71"/>
-      <c r="AF27" s="71"/>
-      <c r="AG27" s="71"/>
-      <c r="AH27" s="71"/>
-      <c r="AI27" s="71"/>
-      <c r="AJ27" s="71"/>
-      <c r="AK27" s="71"/>
-      <c r="AL27" s="71"/>
-      <c r="AM27" s="71"/>
-      <c r="AN27" s="71"/>
-      <c r="AO27" s="71"/>
-      <c r="AP27" s="71"/>
-      <c r="AQ27" s="71"/>
-      <c r="AR27" s="71"/>
-      <c r="AS27" s="71"/>
-      <c r="AT27" s="71"/>
-      <c r="AU27" s="71"/>
-      <c r="AV27" s="71"/>
-      <c r="AW27" s="71"/>
-      <c r="AX27" s="71"/>
-      <c r="AY27" s="71"/>
-      <c r="AZ27" s="71"/>
-      <c r="BA27" s="71"/>
-      <c r="BB27" s="71"/>
-      <c r="BC27" s="71"/>
-      <c r="BD27" s="71"/>
-      <c r="BE27" s="71"/>
-      <c r="BF27" s="71"/>
-      <c r="BG27" s="71"/>
-      <c r="BH27" s="71"/>
-      <c r="BI27" s="71"/>
-      <c r="BJ27" s="71"/>
-      <c r="BK27" s="71"/>
-      <c r="BL27" s="71"/>
-      <c r="BM27" s="71"/>
-      <c r="BN27" s="71"/>
-      <c r="BO27" s="71"/>
+      <c r="M27" s="72"/>
+      <c r="N27" s="72"/>
+      <c r="O27" s="72"/>
+      <c r="P27" s="72"/>
+      <c r="Q27" s="72"/>
+      <c r="R27" s="72"/>
+      <c r="S27" s="72"/>
+      <c r="T27" s="72"/>
+      <c r="U27" s="72"/>
+      <c r="V27" s="72"/>
+      <c r="W27" s="72"/>
+      <c r="X27" s="72"/>
+      <c r="Y27" s="72"/>
+      <c r="Z27" s="72"/>
+      <c r="AA27" s="72"/>
+      <c r="AB27" s="72"/>
+      <c r="AC27" s="72"/>
+      <c r="AD27" s="72"/>
+      <c r="AE27" s="72"/>
+      <c r="AF27" s="72"/>
+      <c r="AG27" s="72"/>
+      <c r="AH27" s="72"/>
+      <c r="AI27" s="72"/>
+      <c r="AJ27" s="72"/>
+      <c r="AK27" s="72"/>
+      <c r="AL27" s="72"/>
+      <c r="AM27" s="72"/>
+      <c r="AN27" s="72"/>
+      <c r="AO27" s="72"/>
+      <c r="AP27" s="72"/>
+      <c r="AQ27" s="72"/>
+      <c r="AR27" s="72"/>
+      <c r="AS27" s="72"/>
+      <c r="AT27" s="72"/>
+      <c r="AU27" s="72"/>
+      <c r="AV27" s="72"/>
+      <c r="AW27" s="72"/>
+      <c r="AX27" s="72"/>
+      <c r="AY27" s="72"/>
+      <c r="AZ27" s="72"/>
+      <c r="BA27" s="72"/>
+      <c r="BB27" s="72"/>
+      <c r="BC27" s="72"/>
+      <c r="BD27" s="72"/>
+      <c r="BE27" s="72"/>
+      <c r="BF27" s="72"/>
+      <c r="BG27" s="72"/>
+      <c r="BH27" s="72"/>
+      <c r="BI27" s="72"/>
+      <c r="BJ27" s="72"/>
+      <c r="BK27" s="72"/>
+      <c r="BL27" s="72"/>
+      <c r="BM27" s="72"/>
+      <c r="BN27" s="72"/>
+      <c r="BO27" s="72"/>
       <c r="BP27" s="16"/>
-      <c r="BQ27" s="58"/>
-      <c r="BR27" s="58"/>
+      <c r="BQ27" s="59"/>
+      <c r="BR27" s="59"/>
       <c r="BS27" s="4"/>
       <c r="BT27" s="6"/>
       <c r="BU27" s="34"/>
@@ -4323,50 +4327,50 @@
       <c r="BN28" s="34"/>
       <c r="BO28" s="34"/>
       <c r="BP28" s="16"/>
-      <c r="BQ28" s="58"/>
-      <c r="BR28" s="58"/>
+      <c r="BQ28" s="59"/>
+      <c r="BR28" s="59"/>
       <c r="BS28" s="4"/>
       <c r="BT28" s="6"/>
-      <c r="BU28" s="72"/>
-      <c r="BV28" s="72"/>
-      <c r="BW28" s="72"/>
-      <c r="BX28" s="72"/>
-      <c r="BY28" s="72"/>
-      <c r="BZ28" s="72"/>
-      <c r="CA28" s="72"/>
-      <c r="CB28" s="72"/>
-      <c r="CC28" s="72"/>
-      <c r="CD28" s="72"/>
-      <c r="CE28" s="72"/>
-      <c r="CF28" s="72"/>
-      <c r="CG28" s="72"/>
-      <c r="CH28" s="72"/>
-      <c r="CI28" s="72"/>
-      <c r="CJ28" s="72"/>
-      <c r="CK28" s="72"/>
-      <c r="CL28" s="72"/>
-      <c r="CM28" s="72"/>
-      <c r="CN28" s="72"/>
-      <c r="CO28" s="72"/>
-      <c r="CP28" s="72"/>
-      <c r="CQ28" s="72"/>
-      <c r="CR28" s="72"/>
-      <c r="CS28" s="72"/>
-      <c r="CT28" s="72"/>
-      <c r="CU28" s="72"/>
-      <c r="CV28" s="72"/>
-      <c r="CW28" s="72"/>
-      <c r="CX28" s="72"/>
-      <c r="CY28" s="72"/>
-      <c r="CZ28" s="72"/>
-      <c r="DA28" s="72"/>
-      <c r="DB28" s="72"/>
-      <c r="DC28" s="72"/>
-      <c r="DD28" s="72"/>
-      <c r="DE28" s="72"/>
-      <c r="DF28" s="72"/>
-      <c r="DG28" s="72"/>
-      <c r="DH28" s="72"/>
+      <c r="BU28" s="73"/>
+      <c r="BV28" s="73"/>
+      <c r="BW28" s="73"/>
+      <c r="BX28" s="73"/>
+      <c r="BY28" s="73"/>
+      <c r="BZ28" s="73"/>
+      <c r="CA28" s="73"/>
+      <c r="CB28" s="73"/>
+      <c r="CC28" s="73"/>
+      <c r="CD28" s="73"/>
+      <c r="CE28" s="73"/>
+      <c r="CF28" s="73"/>
+      <c r="CG28" s="73"/>
+      <c r="CH28" s="73"/>
+      <c r="CI28" s="73"/>
+      <c r="CJ28" s="73"/>
+      <c r="CK28" s="73"/>
+      <c r="CL28" s="73"/>
+      <c r="CM28" s="73"/>
+      <c r="CN28" s="73"/>
+      <c r="CO28" s="73"/>
+      <c r="CP28" s="73"/>
+      <c r="CQ28" s="73"/>
+      <c r="CR28" s="73"/>
+      <c r="CS28" s="73"/>
+      <c r="CT28" s="73"/>
+      <c r="CU28" s="73"/>
+      <c r="CV28" s="73"/>
+      <c r="CW28" s="73"/>
+      <c r="CX28" s="73"/>
+      <c r="CY28" s="73"/>
+      <c r="CZ28" s="73"/>
+      <c r="DA28" s="73"/>
+      <c r="DB28" s="73"/>
+      <c r="DC28" s="73"/>
+      <c r="DD28" s="73"/>
+      <c r="DE28" s="73"/>
+      <c r="DF28" s="73"/>
+      <c r="DG28" s="73"/>
+      <c r="DH28" s="73"/>
       <c r="DI28" s="6"/>
       <c r="DL28" s="56"/>
     </row>
@@ -4380,71 +4384,71 @@
       <c r="E29" s="1"/>
       <c r="F29" s="1"/>
       <c r="G29" s="1"/>
-      <c r="H29" s="62"/>
-      <c r="I29" s="73" t="s">
+      <c r="H29" s="63"/>
+      <c r="I29" s="74" t="s">
         <v>82</v>
       </c>
-      <c r="J29" s="73"/>
-      <c r="K29" s="73"/>
-      <c r="L29" s="73"/>
-      <c r="M29" s="73"/>
-      <c r="N29" s="73"/>
-      <c r="O29" s="73"/>
-      <c r="P29" s="73"/>
-      <c r="Q29" s="73"/>
-      <c r="R29" s="73"/>
-      <c r="S29" s="73"/>
-      <c r="T29" s="73"/>
-      <c r="U29" s="73"/>
-      <c r="V29" s="73"/>
-      <c r="W29" s="73"/>
-      <c r="X29" s="73"/>
-      <c r="Y29" s="73"/>
-      <c r="Z29" s="73"/>
-      <c r="AA29" s="73"/>
-      <c r="AB29" s="73"/>
-      <c r="AC29" s="73"/>
-      <c r="AD29" s="73"/>
-      <c r="AE29" s="73"/>
-      <c r="AF29" s="73"/>
-      <c r="AG29" s="73"/>
-      <c r="AH29" s="73"/>
-      <c r="AI29" s="73"/>
-      <c r="AJ29" s="73"/>
-      <c r="AK29" s="73"/>
-      <c r="AL29" s="73"/>
-      <c r="AM29" s="73"/>
-      <c r="AN29" s="73"/>
-      <c r="AO29" s="73"/>
-      <c r="AP29" s="73"/>
-      <c r="AQ29" s="73"/>
-      <c r="AR29" s="73"/>
-      <c r="AS29" s="73"/>
-      <c r="AT29" s="73"/>
-      <c r="AU29" s="73"/>
-      <c r="AV29" s="73"/>
-      <c r="AW29" s="73"/>
-      <c r="AX29" s="73"/>
-      <c r="AY29" s="73"/>
-      <c r="AZ29" s="73"/>
-      <c r="BA29" s="73"/>
-      <c r="BB29" s="73"/>
-      <c r="BC29" s="73"/>
-      <c r="BD29" s="73"/>
-      <c r="BE29" s="73"/>
-      <c r="BF29" s="73"/>
-      <c r="BG29" s="73"/>
-      <c r="BH29" s="73"/>
-      <c r="BI29" s="73"/>
-      <c r="BJ29" s="73"/>
-      <c r="BK29" s="73"/>
-      <c r="BL29" s="73"/>
-      <c r="BM29" s="73"/>
-      <c r="BN29" s="73"/>
-      <c r="BO29" s="73"/>
+      <c r="J29" s="74"/>
+      <c r="K29" s="74"/>
+      <c r="L29" s="74"/>
+      <c r="M29" s="74"/>
+      <c r="N29" s="74"/>
+      <c r="O29" s="74"/>
+      <c r="P29" s="74"/>
+      <c r="Q29" s="74"/>
+      <c r="R29" s="74"/>
+      <c r="S29" s="74"/>
+      <c r="T29" s="74"/>
+      <c r="U29" s="74"/>
+      <c r="V29" s="74"/>
+      <c r="W29" s="74"/>
+      <c r="X29" s="74"/>
+      <c r="Y29" s="74"/>
+      <c r="Z29" s="74"/>
+      <c r="AA29" s="74"/>
+      <c r="AB29" s="74"/>
+      <c r="AC29" s="74"/>
+      <c r="AD29" s="74"/>
+      <c r="AE29" s="74"/>
+      <c r="AF29" s="74"/>
+      <c r="AG29" s="74"/>
+      <c r="AH29" s="74"/>
+      <c r="AI29" s="74"/>
+      <c r="AJ29" s="74"/>
+      <c r="AK29" s="74"/>
+      <c r="AL29" s="74"/>
+      <c r="AM29" s="74"/>
+      <c r="AN29" s="74"/>
+      <c r="AO29" s="74"/>
+      <c r="AP29" s="74"/>
+      <c r="AQ29" s="74"/>
+      <c r="AR29" s="74"/>
+      <c r="AS29" s="74"/>
+      <c r="AT29" s="74"/>
+      <c r="AU29" s="74"/>
+      <c r="AV29" s="74"/>
+      <c r="AW29" s="74"/>
+      <c r="AX29" s="74"/>
+      <c r="AY29" s="74"/>
+      <c r="AZ29" s="74"/>
+      <c r="BA29" s="74"/>
+      <c r="BB29" s="74"/>
+      <c r="BC29" s="74"/>
+      <c r="BD29" s="74"/>
+      <c r="BE29" s="74"/>
+      <c r="BF29" s="74"/>
+      <c r="BG29" s="74"/>
+      <c r="BH29" s="74"/>
+      <c r="BI29" s="74"/>
+      <c r="BJ29" s="74"/>
+      <c r="BK29" s="74"/>
+      <c r="BL29" s="74"/>
+      <c r="BM29" s="74"/>
+      <c r="BN29" s="74"/>
+      <c r="BO29" s="74"/>
       <c r="BP29" s="16"/>
-      <c r="BQ29" s="58"/>
-      <c r="BR29" s="58"/>
+      <c r="BQ29" s="59"/>
+      <c r="BR29" s="59"/>
       <c r="BS29" s="4"/>
       <c r="BT29" s="6"/>
       <c r="BU29" s="26" t="s">
@@ -4459,38 +4463,38 @@
       <c r="CB29" s="6"/>
       <c r="CC29" s="6"/>
       <c r="CD29" s="6"/>
-      <c r="CE29" s="73" t="n">
+      <c r="CE29" s="74" t="n">
         <v>15</v>
       </c>
-      <c r="CF29" s="73"/>
-      <c r="CG29" s="73"/>
-      <c r="CH29" s="73"/>
-      <c r="CI29" s="73"/>
-      <c r="CJ29" s="73"/>
-      <c r="CK29" s="73"/>
-      <c r="CL29" s="73"/>
-      <c r="CM29" s="73"/>
-      <c r="CN29" s="73"/>
-      <c r="CO29" s="73"/>
-      <c r="CP29" s="73"/>
-      <c r="CQ29" s="73"/>
-      <c r="CR29" s="73"/>
-      <c r="CS29" s="73"/>
-      <c r="CT29" s="73"/>
-      <c r="CU29" s="73"/>
-      <c r="CV29" s="73"/>
-      <c r="CW29" s="73"/>
-      <c r="CX29" s="73"/>
-      <c r="CY29" s="73"/>
-      <c r="CZ29" s="73"/>
-      <c r="DA29" s="73"/>
-      <c r="DB29" s="73"/>
-      <c r="DC29" s="73"/>
-      <c r="DD29" s="73"/>
-      <c r="DE29" s="73"/>
-      <c r="DF29" s="73"/>
-      <c r="DG29" s="73"/>
-      <c r="DH29" s="73"/>
+      <c r="CF29" s="74"/>
+      <c r="CG29" s="74"/>
+      <c r="CH29" s="74"/>
+      <c r="CI29" s="74"/>
+      <c r="CJ29" s="74"/>
+      <c r="CK29" s="74"/>
+      <c r="CL29" s="74"/>
+      <c r="CM29" s="74"/>
+      <c r="CN29" s="74"/>
+      <c r="CO29" s="74"/>
+      <c r="CP29" s="74"/>
+      <c r="CQ29" s="74"/>
+      <c r="CR29" s="74"/>
+      <c r="CS29" s="74"/>
+      <c r="CT29" s="74"/>
+      <c r="CU29" s="74"/>
+      <c r="CV29" s="74"/>
+      <c r="CW29" s="74"/>
+      <c r="CX29" s="74"/>
+      <c r="CY29" s="74"/>
+      <c r="CZ29" s="74"/>
+      <c r="DA29" s="74"/>
+      <c r="DB29" s="74"/>
+      <c r="DC29" s="74"/>
+      <c r="DD29" s="74"/>
+      <c r="DE29" s="74"/>
+      <c r="DF29" s="74"/>
+      <c r="DG29" s="74"/>
+      <c r="DH29" s="74"/>
       <c r="DI29" s="6"/>
       <c r="DL29" s="56"/>
     </row>
@@ -4565,8 +4569,8 @@
       <c r="BN30" s="22"/>
       <c r="BO30" s="22"/>
       <c r="BP30" s="24"/>
-      <c r="BQ30" s="58"/>
-      <c r="BR30" s="58"/>
+      <c r="BQ30" s="59"/>
+      <c r="BR30" s="59"/>
       <c r="BS30" s="12"/>
       <c r="BT30" s="13"/>
       <c r="BU30" s="13"/>
@@ -4681,8 +4685,8 @@
       <c r="BN31" s="34"/>
       <c r="BO31" s="34"/>
       <c r="BP31" s="16"/>
-      <c r="BQ31" s="58"/>
-      <c r="BR31" s="58"/>
+      <c r="BQ31" s="59"/>
+      <c r="BR31" s="59"/>
       <c r="BS31" s="4"/>
       <c r="BT31" s="5"/>
       <c r="BU31" s="5"/>
@@ -4732,79 +4736,79 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.75" outlineLevel="0" r="32">
       <c r="A32" s="6"/>
-      <c r="B32" s="74" t="s">
+      <c r="B32" s="75" t="s">
         <v>85</v>
       </c>
-      <c r="C32" s="74"/>
-      <c r="D32" s="74"/>
-      <c r="E32" s="74"/>
-      <c r="F32" s="74"/>
-      <c r="G32" s="74"/>
-      <c r="H32" s="74"/>
-      <c r="I32" s="74"/>
-      <c r="J32" s="74"/>
-      <c r="K32" s="74"/>
-      <c r="L32" s="75" t="n">
+      <c r="C32" s="75"/>
+      <c r="D32" s="75"/>
+      <c r="E32" s="75"/>
+      <c r="F32" s="75"/>
+      <c r="G32" s="75"/>
+      <c r="H32" s="75"/>
+      <c r="I32" s="75"/>
+      <c r="J32" s="75"/>
+      <c r="K32" s="75"/>
+      <c r="L32" s="76" t="n">
         <v>15</v>
       </c>
-      <c r="M32" s="75"/>
-      <c r="N32" s="75"/>
-      <c r="O32" s="75"/>
-      <c r="P32" s="75"/>
-      <c r="Q32" s="75"/>
-      <c r="R32" s="75"/>
-      <c r="S32" s="75"/>
-      <c r="T32" s="75"/>
-      <c r="U32" s="75"/>
-      <c r="V32" s="75"/>
-      <c r="W32" s="75"/>
-      <c r="X32" s="75"/>
-      <c r="Y32" s="75"/>
-      <c r="Z32" s="75"/>
-      <c r="AA32" s="75"/>
-      <c r="AB32" s="75"/>
-      <c r="AC32" s="75"/>
-      <c r="AD32" s="75"/>
-      <c r="AE32" s="75"/>
-      <c r="AF32" s="75"/>
-      <c r="AG32" s="75"/>
-      <c r="AH32" s="75"/>
-      <c r="AI32" s="75"/>
-      <c r="AJ32" s="75"/>
-      <c r="AK32" s="75"/>
-      <c r="AL32" s="75"/>
-      <c r="AM32" s="75"/>
-      <c r="AN32" s="75"/>
-      <c r="AO32" s="75"/>
-      <c r="AP32" s="75"/>
-      <c r="AQ32" s="75"/>
-      <c r="AR32" s="75"/>
-      <c r="AS32" s="75"/>
-      <c r="AT32" s="75"/>
-      <c r="AU32" s="75"/>
-      <c r="AV32" s="75"/>
-      <c r="AW32" s="75"/>
-      <c r="AX32" s="75"/>
-      <c r="AY32" s="75"/>
-      <c r="AZ32" s="75"/>
-      <c r="BA32" s="75"/>
-      <c r="BB32" s="75"/>
-      <c r="BC32" s="75"/>
-      <c r="BD32" s="75"/>
-      <c r="BE32" s="75"/>
-      <c r="BF32" s="75"/>
-      <c r="BG32" s="75"/>
-      <c r="BH32" s="75"/>
-      <c r="BI32" s="75"/>
-      <c r="BJ32" s="75"/>
-      <c r="BK32" s="75"/>
-      <c r="BL32" s="75"/>
-      <c r="BM32" s="75"/>
-      <c r="BN32" s="75"/>
-      <c r="BO32" s="75"/>
+      <c r="M32" s="76"/>
+      <c r="N32" s="76"/>
+      <c r="O32" s="76"/>
+      <c r="P32" s="76"/>
+      <c r="Q32" s="76"/>
+      <c r="R32" s="76"/>
+      <c r="S32" s="76"/>
+      <c r="T32" s="76"/>
+      <c r="U32" s="76"/>
+      <c r="V32" s="76"/>
+      <c r="W32" s="76"/>
+      <c r="X32" s="76"/>
+      <c r="Y32" s="76"/>
+      <c r="Z32" s="76"/>
+      <c r="AA32" s="76"/>
+      <c r="AB32" s="76"/>
+      <c r="AC32" s="76"/>
+      <c r="AD32" s="76"/>
+      <c r="AE32" s="76"/>
+      <c r="AF32" s="76"/>
+      <c r="AG32" s="76"/>
+      <c r="AH32" s="76"/>
+      <c r="AI32" s="76"/>
+      <c r="AJ32" s="76"/>
+      <c r="AK32" s="76"/>
+      <c r="AL32" s="76"/>
+      <c r="AM32" s="76"/>
+      <c r="AN32" s="76"/>
+      <c r="AO32" s="76"/>
+      <c r="AP32" s="76"/>
+      <c r="AQ32" s="76"/>
+      <c r="AR32" s="76"/>
+      <c r="AS32" s="76"/>
+      <c r="AT32" s="76"/>
+      <c r="AU32" s="76"/>
+      <c r="AV32" s="76"/>
+      <c r="AW32" s="76"/>
+      <c r="AX32" s="76"/>
+      <c r="AY32" s="76"/>
+      <c r="AZ32" s="76"/>
+      <c r="BA32" s="76"/>
+      <c r="BB32" s="76"/>
+      <c r="BC32" s="76"/>
+      <c r="BD32" s="76"/>
+      <c r="BE32" s="76"/>
+      <c r="BF32" s="76"/>
+      <c r="BG32" s="76"/>
+      <c r="BH32" s="76"/>
+      <c r="BI32" s="76"/>
+      <c r="BJ32" s="76"/>
+      <c r="BK32" s="76"/>
+      <c r="BL32" s="76"/>
+      <c r="BM32" s="76"/>
+      <c r="BN32" s="76"/>
+      <c r="BO32" s="76"/>
       <c r="BP32" s="16"/>
-      <c r="BQ32" s="58"/>
-      <c r="BR32" s="58"/>
+      <c r="BQ32" s="59"/>
+      <c r="BR32" s="59"/>
       <c r="BS32" s="4"/>
       <c r="BT32" s="5"/>
       <c r="BU32" s="5"/>
@@ -4862,65 +4866,65 @@
       <c r="I33" s="1"/>
       <c r="J33" s="1"/>
       <c r="K33" s="1"/>
-      <c r="L33" s="75"/>
-      <c r="M33" s="75"/>
-      <c r="N33" s="75"/>
-      <c r="O33" s="75"/>
-      <c r="P33" s="75"/>
-      <c r="Q33" s="75"/>
-      <c r="R33" s="75"/>
-      <c r="S33" s="75"/>
-      <c r="T33" s="75"/>
-      <c r="U33" s="75"/>
-      <c r="V33" s="75"/>
-      <c r="W33" s="75"/>
-      <c r="X33" s="75"/>
-      <c r="Y33" s="75"/>
-      <c r="Z33" s="75"/>
-      <c r="AA33" s="75"/>
-      <c r="AB33" s="75"/>
-      <c r="AC33" s="75"/>
-      <c r="AD33" s="75"/>
-      <c r="AE33" s="75"/>
-      <c r="AF33" s="75"/>
-      <c r="AG33" s="75"/>
-      <c r="AH33" s="75"/>
-      <c r="AI33" s="75"/>
-      <c r="AJ33" s="75"/>
-      <c r="AK33" s="75"/>
-      <c r="AL33" s="75"/>
-      <c r="AM33" s="75"/>
-      <c r="AN33" s="75"/>
-      <c r="AO33" s="75"/>
-      <c r="AP33" s="75"/>
-      <c r="AQ33" s="75"/>
-      <c r="AR33" s="75"/>
-      <c r="AS33" s="75"/>
-      <c r="AT33" s="75"/>
-      <c r="AU33" s="75"/>
-      <c r="AV33" s="75"/>
-      <c r="AW33" s="75"/>
-      <c r="AX33" s="75"/>
-      <c r="AY33" s="75"/>
-      <c r="AZ33" s="75"/>
-      <c r="BA33" s="75"/>
-      <c r="BB33" s="75"/>
-      <c r="BC33" s="75"/>
-      <c r="BD33" s="75"/>
-      <c r="BE33" s="75"/>
-      <c r="BF33" s="75"/>
-      <c r="BG33" s="75"/>
-      <c r="BH33" s="75"/>
-      <c r="BI33" s="75"/>
-      <c r="BJ33" s="75"/>
-      <c r="BK33" s="75"/>
-      <c r="BL33" s="75"/>
-      <c r="BM33" s="75"/>
-      <c r="BN33" s="75"/>
-      <c r="BO33" s="75"/>
+      <c r="L33" s="76"/>
+      <c r="M33" s="76"/>
+      <c r="N33" s="76"/>
+      <c r="O33" s="76"/>
+      <c r="P33" s="76"/>
+      <c r="Q33" s="76"/>
+      <c r="R33" s="76"/>
+      <c r="S33" s="76"/>
+      <c r="T33" s="76"/>
+      <c r="U33" s="76"/>
+      <c r="V33" s="76"/>
+      <c r="W33" s="76"/>
+      <c r="X33" s="76"/>
+      <c r="Y33" s="76"/>
+      <c r="Z33" s="76"/>
+      <c r="AA33" s="76"/>
+      <c r="AB33" s="76"/>
+      <c r="AC33" s="76"/>
+      <c r="AD33" s="76"/>
+      <c r="AE33" s="76"/>
+      <c r="AF33" s="76"/>
+      <c r="AG33" s="76"/>
+      <c r="AH33" s="76"/>
+      <c r="AI33" s="76"/>
+      <c r="AJ33" s="76"/>
+      <c r="AK33" s="76"/>
+      <c r="AL33" s="76"/>
+      <c r="AM33" s="76"/>
+      <c r="AN33" s="76"/>
+      <c r="AO33" s="76"/>
+      <c r="AP33" s="76"/>
+      <c r="AQ33" s="76"/>
+      <c r="AR33" s="76"/>
+      <c r="AS33" s="76"/>
+      <c r="AT33" s="76"/>
+      <c r="AU33" s="76"/>
+      <c r="AV33" s="76"/>
+      <c r="AW33" s="76"/>
+      <c r="AX33" s="76"/>
+      <c r="AY33" s="76"/>
+      <c r="AZ33" s="76"/>
+      <c r="BA33" s="76"/>
+      <c r="BB33" s="76"/>
+      <c r="BC33" s="76"/>
+      <c r="BD33" s="76"/>
+      <c r="BE33" s="76"/>
+      <c r="BF33" s="76"/>
+      <c r="BG33" s="76"/>
+      <c r="BH33" s="76"/>
+      <c r="BI33" s="76"/>
+      <c r="BJ33" s="76"/>
+      <c r="BK33" s="76"/>
+      <c r="BL33" s="76"/>
+      <c r="BM33" s="76"/>
+      <c r="BN33" s="76"/>
+      <c r="BO33" s="76"/>
       <c r="BP33" s="16"/>
-      <c r="BQ33" s="58"/>
-      <c r="BR33" s="58"/>
+      <c r="BQ33" s="59"/>
+      <c r="BR33" s="59"/>
       <c r="BS33" s="4"/>
       <c r="BT33" s="5"/>
       <c r="BU33" s="5"/>
@@ -5035,28 +5039,28 @@
       <c r="BN34" s="14"/>
       <c r="BO34" s="14"/>
       <c r="BP34" s="14"/>
-      <c r="BQ34" s="58"/>
-      <c r="BR34" s="58"/>
+      <c r="BQ34" s="59"/>
+      <c r="BR34" s="59"/>
       <c r="BS34" s="4"/>
       <c r="BT34" s="5"/>
       <c r="BU34" s="5"/>
       <c r="BV34" s="5"/>
       <c r="BW34" s="5"/>
-      <c r="BX34" s="76" t="s">
+      <c r="BX34" s="77" t="s">
         <v>86</v>
       </c>
-      <c r="BY34" s="76"/>
-      <c r="BZ34" s="76"/>
-      <c r="CA34" s="76"/>
-      <c r="CB34" s="76"/>
-      <c r="CC34" s="76"/>
-      <c r="CD34" s="76"/>
-      <c r="CE34" s="76"/>
-      <c r="CF34" s="76"/>
-      <c r="CG34" s="76"/>
-      <c r="CH34" s="76"/>
-      <c r="CI34" s="76"/>
-      <c r="CJ34" s="76"/>
+      <c r="BY34" s="77"/>
+      <c r="BZ34" s="77"/>
+      <c r="CA34" s="77"/>
+      <c r="CB34" s="77"/>
+      <c r="CC34" s="77"/>
+      <c r="CD34" s="77"/>
+      <c r="CE34" s="77"/>
+      <c r="CF34" s="77"/>
+      <c r="CG34" s="77"/>
+      <c r="CH34" s="77"/>
+      <c r="CI34" s="77"/>
+      <c r="CJ34" s="77"/>
       <c r="CK34" s="1"/>
       <c r="CL34" s="1"/>
       <c r="CM34" s="1"/>
@@ -5098,7 +5102,7 @@
       <c r="I35" s="1"/>
       <c r="J35" s="1"/>
       <c r="K35" s="1"/>
-      <c r="L35" s="62"/>
+      <c r="L35" s="63"/>
       <c r="M35" s="34" t="s">
         <v>87</v>
       </c>
@@ -5157,26 +5161,26 @@
       <c r="BN35" s="34"/>
       <c r="BO35" s="34"/>
       <c r="BP35" s="16"/>
-      <c r="BQ35" s="58"/>
-      <c r="BR35" s="58"/>
+      <c r="BQ35" s="59"/>
+      <c r="BR35" s="59"/>
       <c r="BS35" s="4"/>
       <c r="BT35" s="5"/>
       <c r="BU35" s="5"/>
       <c r="BV35" s="5"/>
       <c r="BW35" s="5"/>
-      <c r="BX35" s="76"/>
-      <c r="BY35" s="76"/>
-      <c r="BZ35" s="76"/>
-      <c r="CA35" s="76"/>
-      <c r="CB35" s="76"/>
-      <c r="CC35" s="76"/>
-      <c r="CD35" s="76"/>
-      <c r="CE35" s="76"/>
-      <c r="CF35" s="76"/>
-      <c r="CG35" s="76"/>
-      <c r="CH35" s="76"/>
-      <c r="CI35" s="76"/>
-      <c r="CJ35" s="76"/>
+      <c r="BX35" s="77"/>
+      <c r="BY35" s="77"/>
+      <c r="BZ35" s="77"/>
+      <c r="CA35" s="77"/>
+      <c r="CB35" s="77"/>
+      <c r="CC35" s="77"/>
+      <c r="CD35" s="77"/>
+      <c r="CE35" s="77"/>
+      <c r="CF35" s="77"/>
+      <c r="CG35" s="77"/>
+      <c r="CH35" s="77"/>
+      <c r="CI35" s="77"/>
+      <c r="CJ35" s="77"/>
       <c r="CK35" s="1"/>
       <c r="CL35" s="1"/>
       <c r="CM35" s="1"/>
@@ -5273,8 +5277,8 @@
       <c r="BN36" s="14"/>
       <c r="BO36" s="14"/>
       <c r="BP36" s="14"/>
-      <c r="BQ36" s="58"/>
-      <c r="BR36" s="58"/>
+      <c r="BQ36" s="59"/>
+      <c r="BR36" s="59"/>
       <c r="BS36" s="4"/>
       <c r="BT36" s="5"/>
       <c r="BU36" s="5"/>
@@ -5322,67 +5326,67 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.75" outlineLevel="0" r="37">
       <c r="A37" s="6"/>
-      <c r="B37" s="74" t="s">
+      <c r="B37" s="75" t="s">
         <v>88</v>
       </c>
-      <c r="C37" s="74"/>
-      <c r="D37" s="74"/>
-      <c r="E37" s="74"/>
-      <c r="F37" s="74"/>
-      <c r="G37" s="74"/>
-      <c r="H37" s="74"/>
-      <c r="I37" s="74"/>
-      <c r="J37" s="74"/>
-      <c r="K37" s="74"/>
-      <c r="L37" s="74"/>
-      <c r="M37" s="74"/>
-      <c r="N37" s="74"/>
-      <c r="O37" s="74"/>
-      <c r="P37" s="74"/>
-      <c r="Q37" s="74"/>
-      <c r="R37" s="77"/>
-      <c r="S37" s="77"/>
-      <c r="T37" s="77"/>
-      <c r="U37" s="77"/>
-      <c r="V37" s="77"/>
-      <c r="W37" s="77"/>
-      <c r="X37" s="77"/>
-      <c r="Y37" s="77"/>
-      <c r="Z37" s="77"/>
-      <c r="AA37" s="77"/>
-      <c r="AB37" s="77"/>
-      <c r="AC37" s="77"/>
-      <c r="AD37" s="77"/>
-      <c r="AE37" s="77"/>
-      <c r="AF37" s="77"/>
+      <c r="C37" s="75"/>
+      <c r="D37" s="75"/>
+      <c r="E37" s="75"/>
+      <c r="F37" s="75"/>
+      <c r="G37" s="75"/>
+      <c r="H37" s="75"/>
+      <c r="I37" s="75"/>
+      <c r="J37" s="75"/>
+      <c r="K37" s="75"/>
+      <c r="L37" s="75"/>
+      <c r="M37" s="75"/>
+      <c r="N37" s="75"/>
+      <c r="O37" s="75"/>
+      <c r="P37" s="75"/>
+      <c r="Q37" s="75"/>
+      <c r="R37" s="78"/>
+      <c r="S37" s="78"/>
+      <c r="T37" s="78"/>
+      <c r="U37" s="78"/>
+      <c r="V37" s="78"/>
+      <c r="W37" s="78"/>
+      <c r="X37" s="78"/>
+      <c r="Y37" s="78"/>
+      <c r="Z37" s="78"/>
+      <c r="AA37" s="78"/>
+      <c r="AB37" s="78"/>
+      <c r="AC37" s="78"/>
+      <c r="AD37" s="78"/>
+      <c r="AE37" s="78"/>
+      <c r="AF37" s="78"/>
       <c r="AG37" s="6"/>
       <c r="AH37" s="6"/>
       <c r="AI37" s="6"/>
-      <c r="AJ37" s="77"/>
-      <c r="AK37" s="77"/>
-      <c r="AL37" s="77"/>
-      <c r="AM37" s="77"/>
-      <c r="AN37" s="77"/>
-      <c r="AO37" s="77"/>
-      <c r="AP37" s="77"/>
-      <c r="AQ37" s="77"/>
-      <c r="AR37" s="77"/>
-      <c r="AS37" s="77"/>
-      <c r="AT37" s="77"/>
-      <c r="AU37" s="77"/>
-      <c r="AV37" s="77"/>
-      <c r="AW37" s="77"/>
-      <c r="AX37" s="77"/>
-      <c r="AY37" s="77"/>
-      <c r="AZ37" s="77"/>
-      <c r="BA37" s="77"/>
-      <c r="BB37" s="77"/>
-      <c r="BC37" s="77"/>
-      <c r="BD37" s="77"/>
-      <c r="BE37" s="77"/>
-      <c r="BF37" s="77"/>
-      <c r="BG37" s="77"/>
-      <c r="BH37" s="77"/>
+      <c r="AJ37" s="78"/>
+      <c r="AK37" s="78"/>
+      <c r="AL37" s="78"/>
+      <c r="AM37" s="78"/>
+      <c r="AN37" s="78"/>
+      <c r="AO37" s="78"/>
+      <c r="AP37" s="78"/>
+      <c r="AQ37" s="78"/>
+      <c r="AR37" s="78"/>
+      <c r="AS37" s="78"/>
+      <c r="AT37" s="78"/>
+      <c r="AU37" s="78"/>
+      <c r="AV37" s="78"/>
+      <c r="AW37" s="78"/>
+      <c r="AX37" s="78"/>
+      <c r="AY37" s="78"/>
+      <c r="AZ37" s="78"/>
+      <c r="BA37" s="78"/>
+      <c r="BB37" s="78"/>
+      <c r="BC37" s="78"/>
+      <c r="BD37" s="78"/>
+      <c r="BE37" s="78"/>
+      <c r="BF37" s="78"/>
+      <c r="BG37" s="78"/>
+      <c r="BH37" s="78"/>
       <c r="BI37" s="14"/>
       <c r="BJ37" s="14"/>
       <c r="BK37" s="14"/>
@@ -5391,8 +5395,8 @@
       <c r="BN37" s="14"/>
       <c r="BO37" s="14"/>
       <c r="BP37" s="14"/>
-      <c r="BQ37" s="58"/>
-      <c r="BR37" s="58"/>
+      <c r="BQ37" s="59"/>
+      <c r="BR37" s="59"/>
       <c r="BS37" s="4"/>
       <c r="BT37" s="6"/>
       <c r="BU37" s="26" t="s">
@@ -5413,30 +5417,30 @@
       <c r="CH37" s="6"/>
       <c r="CI37" s="6"/>
       <c r="CJ37" s="6"/>
-      <c r="CK37" s="77"/>
-      <c r="CL37" s="77"/>
-      <c r="CM37" s="77"/>
-      <c r="CN37" s="77"/>
-      <c r="CO37" s="77"/>
-      <c r="CP37" s="77"/>
-      <c r="CQ37" s="77"/>
-      <c r="CR37" s="77"/>
-      <c r="CS37" s="77"/>
+      <c r="CK37" s="78"/>
+      <c r="CL37" s="78"/>
+      <c r="CM37" s="78"/>
+      <c r="CN37" s="78"/>
+      <c r="CO37" s="78"/>
+      <c r="CP37" s="78"/>
+      <c r="CQ37" s="78"/>
+      <c r="CR37" s="78"/>
+      <c r="CS37" s="78"/>
       <c r="CT37" s="6"/>
-      <c r="CU37" s="77"/>
-      <c r="CV37" s="77"/>
-      <c r="CW37" s="77"/>
-      <c r="CX37" s="77"/>
-      <c r="CY37" s="77"/>
-      <c r="CZ37" s="77"/>
-      <c r="DA37" s="77"/>
-      <c r="DB37" s="77"/>
-      <c r="DC37" s="77"/>
-      <c r="DD37" s="77"/>
-      <c r="DE37" s="77"/>
-      <c r="DF37" s="77"/>
-      <c r="DG37" s="77"/>
-      <c r="DH37" s="77"/>
+      <c r="CU37" s="78"/>
+      <c r="CV37" s="78"/>
+      <c r="CW37" s="78"/>
+      <c r="CX37" s="78"/>
+      <c r="CY37" s="78"/>
+      <c r="CZ37" s="78"/>
+      <c r="DA37" s="78"/>
+      <c r="DB37" s="78"/>
+      <c r="DC37" s="78"/>
+      <c r="DD37" s="78"/>
+      <c r="DE37" s="78"/>
+      <c r="DF37" s="78"/>
+      <c r="DG37" s="78"/>
+      <c r="DH37" s="78"/>
       <c r="DI37" s="6"/>
       <c r="DL37" s="56"/>
     </row>
@@ -5458,53 +5462,53 @@
       <c r="O38" s="22"/>
       <c r="P38" s="22"/>
       <c r="Q38" s="22"/>
-      <c r="R38" s="78" t="s">
+      <c r="R38" s="79" t="s">
         <v>89</v>
       </c>
-      <c r="S38" s="78"/>
-      <c r="T38" s="78"/>
-      <c r="U38" s="78"/>
-      <c r="V38" s="78"/>
-      <c r="W38" s="78"/>
-      <c r="X38" s="78"/>
-      <c r="Y38" s="78"/>
-      <c r="Z38" s="78"/>
-      <c r="AA38" s="78"/>
-      <c r="AB38" s="78"/>
-      <c r="AC38" s="78"/>
-      <c r="AD38" s="78"/>
-      <c r="AE38" s="78"/>
-      <c r="AF38" s="78"/>
+      <c r="S38" s="79"/>
+      <c r="T38" s="79"/>
+      <c r="U38" s="79"/>
+      <c r="V38" s="79"/>
+      <c r="W38" s="79"/>
+      <c r="X38" s="79"/>
+      <c r="Y38" s="79"/>
+      <c r="Z38" s="79"/>
+      <c r="AA38" s="79"/>
+      <c r="AB38" s="79"/>
+      <c r="AC38" s="79"/>
+      <c r="AD38" s="79"/>
+      <c r="AE38" s="79"/>
+      <c r="AF38" s="79"/>
       <c r="AG38" s="6"/>
       <c r="AH38" s="6"/>
       <c r="AI38" s="6"/>
-      <c r="AJ38" s="78" t="s">
+      <c r="AJ38" s="79" t="s">
         <v>90</v>
       </c>
-      <c r="AK38" s="78"/>
-      <c r="AL38" s="78"/>
-      <c r="AM38" s="78"/>
-      <c r="AN38" s="78"/>
-      <c r="AO38" s="78"/>
-      <c r="AP38" s="78"/>
-      <c r="AQ38" s="78"/>
-      <c r="AR38" s="78"/>
-      <c r="AS38" s="78"/>
-      <c r="AT38" s="78"/>
-      <c r="AU38" s="78"/>
-      <c r="AV38" s="78"/>
-      <c r="AW38" s="78"/>
-      <c r="AX38" s="78"/>
-      <c r="AY38" s="78"/>
-      <c r="AZ38" s="78"/>
-      <c r="BA38" s="78"/>
-      <c r="BB38" s="78"/>
-      <c r="BC38" s="78"/>
-      <c r="BD38" s="78"/>
-      <c r="BE38" s="78"/>
-      <c r="BF38" s="78"/>
-      <c r="BG38" s="78"/>
-      <c r="BH38" s="78"/>
+      <c r="AK38" s="79"/>
+      <c r="AL38" s="79"/>
+      <c r="AM38" s="79"/>
+      <c r="AN38" s="79"/>
+      <c r="AO38" s="79"/>
+      <c r="AP38" s="79"/>
+      <c r="AQ38" s="79"/>
+      <c r="AR38" s="79"/>
+      <c r="AS38" s="79"/>
+      <c r="AT38" s="79"/>
+      <c r="AU38" s="79"/>
+      <c r="AV38" s="79"/>
+      <c r="AW38" s="79"/>
+      <c r="AX38" s="79"/>
+      <c r="AY38" s="79"/>
+      <c r="AZ38" s="79"/>
+      <c r="BA38" s="79"/>
+      <c r="BB38" s="79"/>
+      <c r="BC38" s="79"/>
+      <c r="BD38" s="79"/>
+      <c r="BE38" s="79"/>
+      <c r="BF38" s="79"/>
+      <c r="BG38" s="79"/>
+      <c r="BH38" s="79"/>
       <c r="BI38" s="11"/>
       <c r="BJ38" s="11"/>
       <c r="BK38" s="11"/>
@@ -5513,8 +5517,8 @@
       <c r="BN38" s="11"/>
       <c r="BO38" s="11"/>
       <c r="BP38" s="11"/>
-      <c r="BQ38" s="58"/>
-      <c r="BR38" s="58"/>
+      <c r="BQ38" s="59"/>
+      <c r="BR38" s="59"/>
       <c r="BS38" s="12"/>
       <c r="BT38" s="13"/>
       <c r="BU38" s="13"/>
@@ -5533,102 +5537,102 @@
       <c r="CH38" s="13"/>
       <c r="CI38" s="13"/>
       <c r="CJ38" s="13"/>
-      <c r="CK38" s="79" t="s">
+      <c r="CK38" s="80" t="s">
         <v>89</v>
       </c>
-      <c r="CL38" s="79"/>
-      <c r="CM38" s="79"/>
-      <c r="CN38" s="79"/>
-      <c r="CO38" s="79"/>
-      <c r="CP38" s="79"/>
-      <c r="CQ38" s="79"/>
-      <c r="CR38" s="79"/>
-      <c r="CS38" s="79"/>
-      <c r="CT38" s="80"/>
-      <c r="CU38" s="81" t="s">
+      <c r="CL38" s="80"/>
+      <c r="CM38" s="80"/>
+      <c r="CN38" s="80"/>
+      <c r="CO38" s="80"/>
+      <c r="CP38" s="80"/>
+      <c r="CQ38" s="80"/>
+      <c r="CR38" s="80"/>
+      <c r="CS38" s="80"/>
+      <c r="CT38" s="81"/>
+      <c r="CU38" s="82" t="s">
         <v>90</v>
       </c>
-      <c r="CV38" s="81"/>
-      <c r="CW38" s="81"/>
-      <c r="CX38" s="81"/>
-      <c r="CY38" s="81"/>
-      <c r="CZ38" s="81"/>
-      <c r="DA38" s="81"/>
-      <c r="DB38" s="81"/>
-      <c r="DC38" s="81"/>
-      <c r="DD38" s="81"/>
-      <c r="DE38" s="81"/>
-      <c r="DF38" s="81"/>
-      <c r="DG38" s="81"/>
-      <c r="DH38" s="81"/>
+      <c r="CV38" s="82"/>
+      <c r="CW38" s="82"/>
+      <c r="CX38" s="82"/>
+      <c r="CY38" s="82"/>
+      <c r="CZ38" s="82"/>
+      <c r="DA38" s="82"/>
+      <c r="DB38" s="82"/>
+      <c r="DC38" s="82"/>
+      <c r="DD38" s="82"/>
+      <c r="DE38" s="82"/>
+      <c r="DF38" s="82"/>
+      <c r="DG38" s="82"/>
+      <c r="DH38" s="82"/>
       <c r="DI38" s="6"/>
       <c r="DL38" s="8"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.75" outlineLevel="0" r="39">
-      <c r="A39" s="62"/>
-      <c r="B39" s="74" t="s">
+      <c r="A39" s="63"/>
+      <c r="B39" s="75" t="s">
         <v>91</v>
       </c>
-      <c r="C39" s="74"/>
-      <c r="D39" s="74"/>
-      <c r="E39" s="74"/>
-      <c r="F39" s="74"/>
-      <c r="G39" s="74"/>
-      <c r="H39" s="74"/>
-      <c r="I39" s="74"/>
-      <c r="J39" s="74"/>
-      <c r="K39" s="74"/>
-      <c r="L39" s="74"/>
-      <c r="M39" s="74"/>
-      <c r="N39" s="74"/>
-      <c r="O39" s="74"/>
-      <c r="P39" s="74"/>
-      <c r="Q39" s="74"/>
-      <c r="R39" s="77"/>
-      <c r="S39" s="77"/>
-      <c r="T39" s="77"/>
-      <c r="U39" s="77"/>
-      <c r="V39" s="77"/>
-      <c r="W39" s="77"/>
-      <c r="X39" s="77"/>
-      <c r="Y39" s="77"/>
-      <c r="Z39" s="77"/>
-      <c r="AA39" s="77"/>
-      <c r="AB39" s="77"/>
-      <c r="AC39" s="77"/>
-      <c r="AD39" s="77"/>
-      <c r="AE39" s="77"/>
-      <c r="AF39" s="77"/>
+      <c r="C39" s="75"/>
+      <c r="D39" s="75"/>
+      <c r="E39" s="75"/>
+      <c r="F39" s="75"/>
+      <c r="G39" s="75"/>
+      <c r="H39" s="75"/>
+      <c r="I39" s="75"/>
+      <c r="J39" s="75"/>
+      <c r="K39" s="75"/>
+      <c r="L39" s="75"/>
+      <c r="M39" s="75"/>
+      <c r="N39" s="75"/>
+      <c r="O39" s="75"/>
+      <c r="P39" s="75"/>
+      <c r="Q39" s="75"/>
+      <c r="R39" s="78"/>
+      <c r="S39" s="78"/>
+      <c r="T39" s="78"/>
+      <c r="U39" s="78"/>
+      <c r="V39" s="78"/>
+      <c r="W39" s="78"/>
+      <c r="X39" s="78"/>
+      <c r="Y39" s="78"/>
+      <c r="Z39" s="78"/>
+      <c r="AA39" s="78"/>
+      <c r="AB39" s="78"/>
+      <c r="AC39" s="78"/>
+      <c r="AD39" s="78"/>
+      <c r="AE39" s="78"/>
+      <c r="AF39" s="78"/>
       <c r="AG39" s="6"/>
       <c r="AH39" s="6"/>
       <c r="AI39" s="6"/>
-      <c r="AJ39" s="82" t="s">
+      <c r="AJ39" s="83" t="s">
         <v>40</v>
       </c>
-      <c r="AK39" s="82"/>
-      <c r="AL39" s="82"/>
-      <c r="AM39" s="82"/>
-      <c r="AN39" s="82"/>
-      <c r="AO39" s="82"/>
-      <c r="AP39" s="82"/>
-      <c r="AQ39" s="82"/>
-      <c r="AR39" s="82"/>
-      <c r="AS39" s="82"/>
-      <c r="AT39" s="82"/>
-      <c r="AU39" s="82"/>
-      <c r="AV39" s="82"/>
-      <c r="AW39" s="82"/>
-      <c r="AX39" s="82"/>
-      <c r="AY39" s="82"/>
-      <c r="AZ39" s="82"/>
-      <c r="BA39" s="82"/>
-      <c r="BB39" s="82"/>
-      <c r="BC39" s="82"/>
-      <c r="BD39" s="82"/>
-      <c r="BE39" s="82"/>
-      <c r="BF39" s="82"/>
-      <c r="BG39" s="82"/>
-      <c r="BH39" s="82"/>
+      <c r="AK39" s="83"/>
+      <c r="AL39" s="83"/>
+      <c r="AM39" s="83"/>
+      <c r="AN39" s="83"/>
+      <c r="AO39" s="83"/>
+      <c r="AP39" s="83"/>
+      <c r="AQ39" s="83"/>
+      <c r="AR39" s="83"/>
+      <c r="AS39" s="83"/>
+      <c r="AT39" s="83"/>
+      <c r="AU39" s="83"/>
+      <c r="AV39" s="83"/>
+      <c r="AW39" s="83"/>
+      <c r="AX39" s="83"/>
+      <c r="AY39" s="83"/>
+      <c r="AZ39" s="83"/>
+      <c r="BA39" s="83"/>
+      <c r="BB39" s="83"/>
+      <c r="BC39" s="83"/>
+      <c r="BD39" s="83"/>
+      <c r="BE39" s="83"/>
+      <c r="BF39" s="83"/>
+      <c r="BG39" s="83"/>
+      <c r="BH39" s="83"/>
       <c r="BI39" s="14"/>
       <c r="BJ39" s="14"/>
       <c r="BK39" s="14"/>
@@ -5637,8 +5641,8 @@
       <c r="BN39" s="14"/>
       <c r="BO39" s="14"/>
       <c r="BP39" s="14"/>
-      <c r="BQ39" s="58"/>
-      <c r="BR39" s="58"/>
+      <c r="BQ39" s="59"/>
+      <c r="BR39" s="59"/>
       <c r="BS39" s="4"/>
       <c r="BT39" s="6"/>
       <c r="BU39" s="26" t="s">
@@ -5650,39 +5654,39 @@
       <c r="BY39" s="6"/>
       <c r="BZ39" s="6"/>
       <c r="CA39" s="6"/>
-      <c r="CB39" s="77"/>
-      <c r="CC39" s="77"/>
-      <c r="CD39" s="77"/>
-      <c r="CE39" s="77"/>
-      <c r="CF39" s="77"/>
-      <c r="CG39" s="77"/>
-      <c r="CH39" s="77"/>
-      <c r="CI39" s="77"/>
-      <c r="CJ39" s="77"/>
+      <c r="CB39" s="78"/>
+      <c r="CC39" s="78"/>
+      <c r="CD39" s="78"/>
+      <c r="CE39" s="78"/>
+      <c r="CF39" s="78"/>
+      <c r="CG39" s="78"/>
+      <c r="CH39" s="78"/>
+      <c r="CI39" s="78"/>
+      <c r="CJ39" s="78"/>
       <c r="CK39" s="6"/>
-      <c r="CL39" s="82" t="s">
+      <c r="CL39" s="83" t="s">
         <v>40</v>
       </c>
-      <c r="CM39" s="82"/>
-      <c r="CN39" s="82"/>
-      <c r="CO39" s="82"/>
-      <c r="CP39" s="82"/>
-      <c r="CQ39" s="82"/>
-      <c r="CR39" s="82"/>
-      <c r="CS39" s="82"/>
-      <c r="CT39" s="82"/>
-      <c r="CU39" s="82"/>
-      <c r="CV39" s="82"/>
-      <c r="CW39" s="82"/>
-      <c r="CX39" s="82"/>
-      <c r="CY39" s="82"/>
-      <c r="CZ39" s="82"/>
-      <c r="DA39" s="82"/>
-      <c r="DB39" s="82"/>
-      <c r="DC39" s="82"/>
-      <c r="DD39" s="82"/>
-      <c r="DE39" s="82"/>
-      <c r="DF39" s="82"/>
+      <c r="CM39" s="83"/>
+      <c r="CN39" s="83"/>
+      <c r="CO39" s="83"/>
+      <c r="CP39" s="83"/>
+      <c r="CQ39" s="83"/>
+      <c r="CR39" s="83"/>
+      <c r="CS39" s="83"/>
+      <c r="CT39" s="83"/>
+      <c r="CU39" s="83"/>
+      <c r="CV39" s="83"/>
+      <c r="CW39" s="83"/>
+      <c r="CX39" s="83"/>
+      <c r="CY39" s="83"/>
+      <c r="CZ39" s="83"/>
+      <c r="DA39" s="83"/>
+      <c r="DB39" s="83"/>
+      <c r="DC39" s="83"/>
+      <c r="DD39" s="83"/>
+      <c r="DE39" s="83"/>
+      <c r="DF39" s="83"/>
       <c r="DG39" s="1"/>
       <c r="DH39" s="1"/>
       <c r="DI39" s="6"/>
@@ -5706,53 +5710,53 @@
       <c r="O40" s="22"/>
       <c r="P40" s="22"/>
       <c r="Q40" s="22"/>
-      <c r="R40" s="78" t="s">
+      <c r="R40" s="79" t="s">
         <v>89</v>
       </c>
-      <c r="S40" s="78"/>
-      <c r="T40" s="78"/>
-      <c r="U40" s="78"/>
-      <c r="V40" s="78"/>
-      <c r="W40" s="78"/>
-      <c r="X40" s="78"/>
-      <c r="Y40" s="78"/>
-      <c r="Z40" s="78"/>
-      <c r="AA40" s="78"/>
-      <c r="AB40" s="78"/>
-      <c r="AC40" s="78"/>
-      <c r="AD40" s="78"/>
-      <c r="AE40" s="78"/>
-      <c r="AF40" s="78"/>
+      <c r="S40" s="79"/>
+      <c r="T40" s="79"/>
+      <c r="U40" s="79"/>
+      <c r="V40" s="79"/>
+      <c r="W40" s="79"/>
+      <c r="X40" s="79"/>
+      <c r="Y40" s="79"/>
+      <c r="Z40" s="79"/>
+      <c r="AA40" s="79"/>
+      <c r="AB40" s="79"/>
+      <c r="AC40" s="79"/>
+      <c r="AD40" s="79"/>
+      <c r="AE40" s="79"/>
+      <c r="AF40" s="79"/>
       <c r="AG40" s="6"/>
       <c r="AH40" s="6"/>
       <c r="AI40" s="6"/>
-      <c r="AJ40" s="78" t="s">
+      <c r="AJ40" s="79" t="s">
         <v>90</v>
       </c>
-      <c r="AK40" s="78"/>
-      <c r="AL40" s="78"/>
-      <c r="AM40" s="78"/>
-      <c r="AN40" s="78"/>
-      <c r="AO40" s="78"/>
-      <c r="AP40" s="78"/>
-      <c r="AQ40" s="78"/>
-      <c r="AR40" s="78"/>
-      <c r="AS40" s="78"/>
-      <c r="AT40" s="78"/>
-      <c r="AU40" s="78"/>
-      <c r="AV40" s="78"/>
-      <c r="AW40" s="78"/>
-      <c r="AX40" s="78"/>
-      <c r="AY40" s="78"/>
-      <c r="AZ40" s="78"/>
-      <c r="BA40" s="78"/>
-      <c r="BB40" s="78"/>
-      <c r="BC40" s="78"/>
-      <c r="BD40" s="78"/>
-      <c r="BE40" s="78"/>
-      <c r="BF40" s="78"/>
-      <c r="BG40" s="78"/>
-      <c r="BH40" s="78"/>
+      <c r="AK40" s="79"/>
+      <c r="AL40" s="79"/>
+      <c r="AM40" s="79"/>
+      <c r="AN40" s="79"/>
+      <c r="AO40" s="79"/>
+      <c r="AP40" s="79"/>
+      <c r="AQ40" s="79"/>
+      <c r="AR40" s="79"/>
+      <c r="AS40" s="79"/>
+      <c r="AT40" s="79"/>
+      <c r="AU40" s="79"/>
+      <c r="AV40" s="79"/>
+      <c r="AW40" s="79"/>
+      <c r="AX40" s="79"/>
+      <c r="AY40" s="79"/>
+      <c r="AZ40" s="79"/>
+      <c r="BA40" s="79"/>
+      <c r="BB40" s="79"/>
+      <c r="BC40" s="79"/>
+      <c r="BD40" s="79"/>
+      <c r="BE40" s="79"/>
+      <c r="BF40" s="79"/>
+      <c r="BG40" s="79"/>
+      <c r="BH40" s="79"/>
       <c r="BI40" s="11"/>
       <c r="BJ40" s="11"/>
       <c r="BK40" s="11"/>
@@ -5761,8 +5765,8 @@
       <c r="BN40" s="11"/>
       <c r="BO40" s="11"/>
       <c r="BP40" s="11"/>
-      <c r="BQ40" s="58"/>
-      <c r="BR40" s="58"/>
+      <c r="BQ40" s="59"/>
+      <c r="BR40" s="59"/>
       <c r="BS40" s="12"/>
       <c r="BT40" s="13"/>
       <c r="BU40" s="13"/>
@@ -5772,41 +5776,41 @@
       <c r="BY40" s="13"/>
       <c r="BZ40" s="13"/>
       <c r="CA40" s="13"/>
-      <c r="CB40" s="78" t="s">
+      <c r="CB40" s="79" t="s">
         <v>89</v>
       </c>
-      <c r="CC40" s="78"/>
-      <c r="CD40" s="78"/>
-      <c r="CE40" s="78"/>
-      <c r="CF40" s="78"/>
-      <c r="CG40" s="78"/>
-      <c r="CH40" s="78"/>
-      <c r="CI40" s="78"/>
-      <c r="CJ40" s="78"/>
-      <c r="CK40" s="83"/>
-      <c r="CL40" s="78" t="s">
+      <c r="CC40" s="79"/>
+      <c r="CD40" s="79"/>
+      <c r="CE40" s="79"/>
+      <c r="CF40" s="79"/>
+      <c r="CG40" s="79"/>
+      <c r="CH40" s="79"/>
+      <c r="CI40" s="79"/>
+      <c r="CJ40" s="79"/>
+      <c r="CK40" s="84"/>
+      <c r="CL40" s="79" t="s">
         <v>90</v>
       </c>
-      <c r="CM40" s="78"/>
-      <c r="CN40" s="78"/>
-      <c r="CO40" s="78"/>
-      <c r="CP40" s="78"/>
-      <c r="CQ40" s="78"/>
-      <c r="CR40" s="78"/>
-      <c r="CS40" s="78"/>
-      <c r="CT40" s="78"/>
-      <c r="CU40" s="78"/>
-      <c r="CV40" s="78"/>
-      <c r="CW40" s="78"/>
-      <c r="CX40" s="78"/>
-      <c r="CY40" s="78"/>
-      <c r="CZ40" s="78"/>
-      <c r="DA40" s="78"/>
-      <c r="DB40" s="78"/>
-      <c r="DC40" s="78"/>
-      <c r="DD40" s="78"/>
-      <c r="DE40" s="78"/>
-      <c r="DF40" s="78"/>
+      <c r="CM40" s="79"/>
+      <c r="CN40" s="79"/>
+      <c r="CO40" s="79"/>
+      <c r="CP40" s="79"/>
+      <c r="CQ40" s="79"/>
+      <c r="CR40" s="79"/>
+      <c r="CS40" s="79"/>
+      <c r="CT40" s="79"/>
+      <c r="CU40" s="79"/>
+      <c r="CV40" s="79"/>
+      <c r="CW40" s="79"/>
+      <c r="CX40" s="79"/>
+      <c r="CY40" s="79"/>
+      <c r="CZ40" s="79"/>
+      <c r="DA40" s="79"/>
+      <c r="DB40" s="79"/>
+      <c r="DC40" s="79"/>
+      <c r="DD40" s="79"/>
+      <c r="DE40" s="79"/>
+      <c r="DF40" s="79"/>
       <c r="DG40" s="22"/>
       <c r="DH40" s="22"/>
       <c r="DI40" s="6"/>
@@ -5995,7 +5999,7 @@
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.6666666666667"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.7843137254902"/>
   </cols>
   <sheetData/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -6022,7 +6026,7 @@
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.6666666666667"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.7843137254902"/>
   </cols>
   <sheetData/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>